<commit_message>
Clean up project structure and update outputs
Removed temporary, diagnostic, and redundant documentation files; added CLEANUP_SUMMARY.md and OVERVIEW.md for consolidated documentation. Updated filtered data and output files, including new author and plot outputs. Fixed author metrics export in run_bibliometric_analysis.R to use correct data object.
</commit_message>
<xml_diff>
--- a/literature review/reproducible-bibliometric-analysis/output/Full_Bibliometric_Report.xlsx
+++ b/literature review/reproducible-bibliometric-analysis/output/Full_Bibliometric_Report.xlsx
@@ -10,7 +10,8 @@
     <sheet name="Main Info" sheetId="1" r:id="rId1"/>
     <sheet name="Annual Production" sheetId="2" r:id="rId2"/>
     <sheet name="Most Rel Sources" sheetId="3" r:id="rId3"/>
-    <sheet name="Most Cited Docs" sheetId="4" r:id="rId4"/>
+    <sheet name="Most Rel Authors" sheetId="4" r:id="rId4"/>
+    <sheet name="Most Cited Docs" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -1079,6 +1080,481 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" s="1" customFormat="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Authors       </t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Articles</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Authors       </t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Articles Fractionalized</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CHANG J-S          </t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">ZHU L         </t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>2.167</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CHEN W-H           </t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">MALCATA FX    </t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>1.792</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">MALCATA FX         </t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">KUMAR A       </t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>1.125</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">ZHU L              </t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>FALFUSHYNSKA H</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>1.000</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">HO S-H             </t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">NARAYANAN M   </t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>1.000</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">LAM MK             </t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">OLTRA C       </t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>1.000</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t xml:space="preserve">LIM JUN WEI        </t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t xml:space="preserve">SINGH J       </t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>1.000</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">LIU J              </t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">VAN BEILEN JB </t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>1.000</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">SHOW PAU LOKE      </t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">SEN R         </t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>0.833</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t xml:space="preserve">SHOW PL            </t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CHANG J-S     </t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>0.787</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t xml:space="preserve">WANG J             </t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t xml:space="preserve">LAM MK        </t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>0.754</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t xml:space="preserve">WANG Y             </t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t xml:space="preserve">SINGH B       </t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>0.750</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>ABOMOHRA ABDELFATAH</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t xml:space="preserve">AMARO HM      </t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>0.667</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t xml:space="preserve">ABREU M            </t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CHEN Y        </t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>0.667</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t xml:space="preserve">AMARO HM           </t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t xml:space="preserve">MISHRA S      </t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>0.667</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAETANO N          </t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t xml:space="preserve">SIALVE B      </t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>0.667</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CALIJURI ML        </t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t xml:space="preserve">VERMA AK      </t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>0.667</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CHEN H             </t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t xml:space="preserve">KUMAR L       </t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>0.625</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CHEN Y             </t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t xml:space="preserve">HO S-H        </t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>0.587</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CHEW KW            </t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAETANO N     </t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>0.583</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>